<commit_message>
Updates for Okanogan Limiting Facotrs, added Yakama Fisheries Logo, etc.
</commit_message>
<xml_diff>
--- a/Data/Okanogan_EDT/AttributeCrosswalk_Okanogan_EDT.xlsx
+++ b/Data/Okanogan_EDT/AttributeCrosswalk_Okanogan_EDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Okanogan_EDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218360AC-3652-4832-BCE5-C5E693E9B183}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E34C8FD-5E96-47E9-92B5-15945C07A12C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1452" windowWidth="17820" windowHeight="11508" xr2:uid="{18FB9C3A-36BA-4F56-919C-AFFAD8A1DF30}"/>
+    <workbookView xWindow="4560" yWindow="972" windowWidth="21984" windowHeight="11544" xr2:uid="{18FB9C3A-36BA-4F56-919C-AFFAD8A1DF30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
   <si>
     <t>Level 3 Attribute</t>
   </si>
@@ -315,7 +315,13 @@
     <t>Woody Debris</t>
   </si>
   <si>
-    <t>Riparian_Mean</t>
+    <t>HQ Pathway Attribute?</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Riparian</t>
   </si>
 </sst>
 </file>
@@ -600,24 +606,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{05955A19-8A5C-4B73-A319-5563E6D05EC4}" name="HabitatAttribute" displayName="HabitatAttribute" ref="B1:C44" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B1:C44" xr:uid="{3CD3C1C8-9CA4-4C09-99D5-1B5A9905A094}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C44">
-    <sortCondition ref="C1:C44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{901011B0-FE84-4A76-BE9F-FED2E5630419}" name="HabitatAttribute4" displayName="HabitatAttribute4" ref="A1:B44" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:B44" xr:uid="{0D54DB80-D62E-4851-8818-237B9BE49FF3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B44">
+    <sortCondition ref="A1:A44"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E0943835-8004-44D0-B0A6-3AC07BFDA62A}" name="Level 2 Attribute" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{65B2D2C9-E455-4620-8E5C-7C1197CE16EF}" name="RTT Habitat Attributes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F6B88623-8165-4267-99FB-D2138C5A93CC}" name="Level 2 Attribute" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1CA7301C-8281-4269-99F1-9CDE5F053D78}" name="RTT Habitat Attributes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{164C4E10-83D0-4C5C-AA7B-5E77CC6B30B5}" name="Level3HabitatAttribute" displayName="Level3HabitatAttribute" ref="A1:A26" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:A26" xr:uid="{A0EC4D5F-F83E-4C26-8925-866BAF1027EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{81D86FFD-2ED6-4AEC-B00E-B2218CDADED3}" name="Level3HabitatAttribute5" displayName="Level3HabitatAttribute5" ref="E1:E26" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="E1:E26" xr:uid="{64725F4F-4B80-4CD2-A59E-3A86C8F88740}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1AE2F564-C8CF-4C16-8EEB-A767E5256DEA}" name="Level 3 Attribute" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{40E58BD4-4B4E-4875-A108-9960886BA9DC}" name="Level 3 Attribute" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -920,505 +926,566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9816DD8-5CB4-4491-8B3E-A6F3CE9F4676}">
-  <dimension ref="A1:D2176"/>
+  <dimension ref="A1:E2176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" style="3" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="3" customWidth="1"/>
     <col min="4" max="4" width="44.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="B28" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="B30" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B31" s="3" t="s">
-        <v>39</v>
+        <v>95</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="B32" s="3" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="B33" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="B34" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="3" t="s">
-        <v>54</v>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="3" t="s">
-        <v>57</v>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
-        <v>63</v>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
-        <v>66</v>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="3" t="s">
-        <v>84</v>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="3" t="s">
-        <v>86</v>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="B42" s="3" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="B43" s="3" t="s">
-        <v>88</v>
+        <v>40</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="B44" s="3" t="s">
-        <v>89</v>
+        <v>32</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
@@ -7806,15 +7873,12 @@
       <c r="D2176" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{26850400-C123-40D9-8A67-949065715850}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{FF4EE0E6-159C-469C-BC51-017876319733}">
       <formula1>$D$2:$D$32</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C36 C39:C45" xr:uid="{4B288D9A-86AD-49DA-8F25-5E35AFBE2DE5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C45 B39:B45 B3:B36" xr:uid="{DACBCFB6-C582-42F5-98B7-7D2B62B9262B}">
       <formula1>$D$2:$D$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4" xr:uid="{513B389A-4EA4-4397-A2EE-D0896503DF2B}">
-      <formula1>$D$2:$D$25</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>